<commit_message>
fix(kb_bootstrap_program): reps not dates
Some of the reps that I'd entered had been interpreted as dates by Calc,
so I needed to go through and ensure they are treated as literal text
instead. I've also put the formula for counting reps against each Learn
row to make it straightforward to extend.
</commit_message>
<xml_diff>
--- a/src/kb/kb_bootstrap_program.xlsx
+++ b/src/kb/kb_bootstrap_program.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="294">
   <si>
     <t xml:space="preserve">Session</t>
   </si>
@@ -147,7 +147,13 @@
     <t xml:space="preserve">Clean, Press</t>
   </si>
   <si>
+    <t xml:space="preserve">6/6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3/3</t>
   </si>
   <si>
     <t xml:space="preserve">8.1</t>
@@ -1319,9 +1325,9 @@
   <dimension ref="A1:AC1005"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F61" activeCellId="0" sqref="F61"/>
+      <selection pane="bottomLeft" activeCell="H76" activeCellId="0" sqref="H76:J76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2148,8 +2154,8 @@
       <c r="H36" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I36" s="18" t="n">
-        <v>45051</v>
+      <c r="I36" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J36" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H36*SUM(SPLIT(I36,""/""))"),20)</f>
@@ -2261,8 +2267,8 @@
       <c r="H41" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I41" s="18" t="n">
-        <v>45209</v>
+      <c r="I41" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="J41" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H41*SUM(SPLIT(I41,""/""))"),40)</f>
@@ -2303,8 +2309,8 @@
       <c r="H43" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I43" s="18" t="n">
-        <v>45051</v>
+      <c r="I43" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J43" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H43*SUM(SPLIT(I43,""/""))"),10)</f>
@@ -2324,8 +2330,8 @@
       <c r="H44" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I44" s="18" t="n">
-        <v>45051</v>
+      <c r="I44" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J44" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H44*SUM(SPLIT(I44,""/""))"),10)</f>
@@ -2366,8 +2372,8 @@
       <c r="H46" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="I46" s="18" t="n">
-        <v>45083</v>
+      <c r="I46" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="J46" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H46*SUM(SPLIT(I46,""/""))"),120)</f>
@@ -2382,13 +2388,13 @@
         <v>38</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H47" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I47" s="18" t="n">
-        <v>44988</v>
+      <c r="I47" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="J47" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H47*SUM(SPLIT(I47,""/""))"),6)</f>
@@ -2479,8 +2485,8 @@
       <c r="H51" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I51" s="18" t="n">
-        <v>45209</v>
+      <c r="I51" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="J51" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H51*SUM(SPLIT(I51,""/""))"),40)</f>
@@ -2500,8 +2506,8 @@
       <c r="H52" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I52" s="18" t="n">
-        <v>45051</v>
+      <c r="I52" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J52" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H52*SUM(SPLIT(I52,""/""))"),20)</f>
@@ -2644,7 +2650,7 @@
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E59" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F59" s="10" t="s">
         <v>18</v>
@@ -2655,8 +2661,8 @@
       <c r="H59" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I59" s="18" t="n">
-        <v>45209</v>
+      <c r="I59" s="18" t="s">
+        <v>30</v>
       </c>
       <c r="J59" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H59*SUM(SPLIT(I59,""/""))"),40)</f>
@@ -2665,7 +2671,7 @@
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E60" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F60" s="10" t="s">
         <v>24</v>
@@ -2686,7 +2692,7 @@
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E61" s="9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F61" s="17" t="s">
         <v>32</v>
@@ -2697,8 +2703,8 @@
       <c r="H61" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I61" s="18" t="n">
-        <v>45051</v>
+      <c r="I61" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J61" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H61*SUM(SPLIT(I61,""/""))"),10)</f>
@@ -2707,7 +2713,7 @@
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E62" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F62" s="17" t="s">
         <v>35</v>
@@ -2718,8 +2724,8 @@
       <c r="H62" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I62" s="18" t="n">
-        <v>45051</v>
+      <c r="I62" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="J62" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H62*SUM(SPLIT(I62,""/""))"),10)</f>
@@ -2728,7 +2734,7 @@
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E63" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F63" s="10" t="s">
         <v>23</v>
@@ -2749,7 +2755,7 @@
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E64" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F64" s="17" t="s">
         <v>37</v>
@@ -2760,8 +2766,8 @@
       <c r="H64" s="13" t="n">
         <v>10</v>
       </c>
-      <c r="I64" s="18" t="n">
-        <v>45083</v>
+      <c r="I64" s="18" t="s">
+        <v>40</v>
       </c>
       <c r="J64" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H64*SUM(SPLIT(I64,""/""))"),120)</f>
@@ -2770,19 +2776,19 @@
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E65" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>38</v>
       </c>
       <c r="G65" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H65" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="I65" s="18" t="n">
-        <v>44988</v>
+      <c r="I65" s="18" t="s">
+        <v>42</v>
       </c>
       <c r="J65" s="13" t="n">
         <f aca="false">IFERROR(__xludf.dummyfunction("H65*SUM(SPLIT(I65,""/""))"),12)</f>
@@ -2803,13 +2809,13 @@
         <v>0</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E67" s="6" t="n">
         <v>9</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
@@ -2840,7 +2846,7 @@
         <v>9.1</v>
       </c>
       <c r="F68" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G68" s="11" t="s">
         <v>13</v>
@@ -2852,96 +2858,160 @@
         <v>9.2</v>
       </c>
       <c r="F69" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G69" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I69" s="9"/>
+      <c r="H69" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I69" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E70" s="3" t="n">
         <v>9.3</v>
       </c>
       <c r="F70" s="17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G70" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I70" s="9"/>
+      <c r="H70" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I70" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E71" s="3" t="n">
         <v>9.4</v>
       </c>
       <c r="F71" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I71" s="9"/>
+      <c r="H71" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E72" s="3" t="n">
         <v>9.5</v>
       </c>
       <c r="F72" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G72" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I72" s="9"/>
+      <c r="H72" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I72" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E73" s="3" t="n">
         <v>9.6</v>
       </c>
       <c r="F73" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G73" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I73" s="9"/>
+      <c r="H73" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E74" s="3" t="n">
         <v>9.7</v>
       </c>
       <c r="F74" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G74" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I74" s="9"/>
+      <c r="H74" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E75" s="3" t="n">
         <v>9.8</v>
       </c>
       <c r="F75" s="17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G75" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I75" s="9"/>
+      <c r="H75" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E76" s="3" t="n">
         <v>9.9</v>
       </c>
       <c r="F76" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G76" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I76" s="9"/>
+      <c r="H76" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="I76" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I77" s="9"/>
@@ -5753,7 +5823,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="D57" activeCellId="1" sqref="H76:J76 D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5766,37 +5836,37 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="K1" s="22" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -5822,10 +5892,10 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="23" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C2" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B2,""\n"",FALSE))"),"Two Hand Deadlift")</f>
@@ -5840,26 +5910,26 @@
         <v>C&amp;P, Sw, Sq</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H2" s="23"/>
       <c r="I2" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J2" s="23"/>
       <c r="K2" s="24" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C3" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B3,""\n"",FALSE))"),"Two Hand Swing")</f>
@@ -5874,24 +5944,24 @@
         <v>C&amp;P, Sw</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
       <c r="K3" s="24" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C4" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B4,""\n"",FALSE))"),"Around the World")</f>
@@ -5910,18 +5980,18 @@
       <c r="H4" s="23"/>
       <c r="I4" s="23"/>
       <c r="J4" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C5" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B5,""\n"",FALSE))"),"Halo")</f>
@@ -5940,18 +6010,18 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C6" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B6,""\n"",FALSE))"),"Around the World Front to Back")</f>
@@ -5970,18 +6040,18 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C7" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B7,""\n"",FALSE))"),"Around the World Back to Front")</f>
@@ -6000,18 +6070,18 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C8" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B8,""\n"",FALSE))"),"Alternating Halo")</f>
@@ -6030,18 +6100,18 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C9" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B9,""\n"",FALSE))"),"Two Hand Pickup One Hand Putdown")</f>
@@ -6056,22 +6126,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="23"/>
       <c r="K9" s="24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C10" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B10,""\n"",FALSE))"),"Single Arm Swing")</f>
@@ -6086,24 +6156,24 @@
         <v>C&amp;P, Sw</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G10" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="23"/>
       <c r="J10" s="23"/>
       <c r="K10" s="24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C11" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B11,""\n"",FALSE))"),"Hand to Hand Transition")</f>
@@ -6118,24 +6188,24 @@
         <v>C&amp;P, Sw</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G11" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="23"/>
       <c r="J11" s="23"/>
       <c r="K11" s="24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C12" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B12,""\n"",FALSE))"),"Two Hand Pickup Clean Putdown")</f>
@@ -6150,22 +6220,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="23"/>
       <c r="J12" s="23"/>
       <c r="K12" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="23" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C13" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B13,""\n"",FALSE))"),"Swing Clean")</f>
@@ -6180,22 +6250,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="23"/>
       <c r="J13" s="23"/>
       <c r="K13" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C14" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B14,""\n"",FALSE))"),"Clean with Hand Transition")</f>
@@ -6210,22 +6280,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
       <c r="I14" s="23"/>
       <c r="J14" s="23"/>
       <c r="K14" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C15" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B15,""\n"",FALSE))"),"Single Arm Overhead Press")</f>
@@ -6240,22 +6310,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F15" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="23"/>
       <c r="I15" s="23"/>
       <c r="J15" s="23"/>
       <c r="K15" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C16" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B16,""\n"",FALSE))"),"Newspaper drill")</f>
@@ -6270,22 +6340,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F16" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
       <c r="J16" s="23"/>
       <c r="K16" s="24" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C17" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B17,""\n"",FALSE))"),"Start Stop Clean")</f>
@@ -6300,22 +6370,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G17" s="23"/>
       <c r="H17" s="23"/>
       <c r="I17" s="23"/>
       <c r="J17" s="23"/>
       <c r="K17" s="24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C18" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B18,""\n"",FALSE))"),"Clean &amp; Press")</f>
@@ -6330,22 +6400,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
       <c r="J18" s="23"/>
       <c r="K18" s="24" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C19" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B19,""\n"",FALSE))"),"Clean &amp; Press with Hand Transition")</f>
@@ -6360,22 +6430,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
       <c r="K19" s="24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C20" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B20,""\n"",FALSE))"),"Start Stop Clean &amp; Press")</f>
@@ -6390,22 +6460,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C21" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B21,""\n"",FALSE))"),"Bottoms-Up Goblet Box Squat")</f>
@@ -6423,19 +6493,19 @@
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
       <c r="I21" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J21" s="23"/>
       <c r="K21" s="24" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C22" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B22,""\n"",FALSE))"),"Goblet Box Squat with Halo")</f>
@@ -6453,21 +6523,21 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K22" s="24" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="23" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C23" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B23,""\n"",FALSE))"),"Goblet Squat with Halo")</f>
@@ -6485,21 +6555,21 @@
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="23" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C24" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B24,""\n"",FALSE))"),"Single-Bell Front Squat")</f>
@@ -6517,19 +6587,19 @@
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J24" s="23"/>
       <c r="K24" s="24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C25" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B25,""\n"",FALSE))"),"Rack Opposite Leg Step-Back Lunge")</f>
@@ -6546,20 +6616,20 @@
       <c r="F25" s="23"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I25" s="23"/>
       <c r="J25" s="23"/>
       <c r="K25" s="24" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="23" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C26" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B26,""\n"",FALSE))"),"Clean Step-Back Clean")</f>
@@ -6576,20 +6646,20 @@
       <c r="F26" s="23"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I26" s="23"/>
       <c r="J26" s="23"/>
       <c r="K26" s="24" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="23" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C27" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B27,""\n"",FALSE))"),"Half-Kneeling Clean")</f>
@@ -6606,20 +6676,20 @@
       <c r="F27" s="23"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I27" s="23"/>
       <c r="J27" s="23"/>
       <c r="K27" s="24" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="23" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C28" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B28,""\n"",FALSE))"),"Clean Step-Back Lunge Clean")</f>
@@ -6634,22 +6704,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F28" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
       <c r="J28" s="23"/>
       <c r="K28" s="24" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="23" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C29" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B29,""\n"",FALSE))"),"Single-Bell Floor Press")</f>
@@ -6666,20 +6736,20 @@
       <c r="F29" s="23"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I29" s="23"/>
       <c r="J29" s="23"/>
       <c r="K29" s="24" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C30" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B30,""\n"",FALSE))"),"Half-Kneeling Clean &amp; Press")</f>
@@ -6694,22 +6764,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G30" s="23"/>
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
       <c r="J30" s="23"/>
       <c r="K30" s="24" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="23" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C31" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B31,""\n"",FALSE))"),"Floor Press with Roll")</f>
@@ -6726,20 +6796,20 @@
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I31" s="23"/>
       <c r="J31" s="23"/>
       <c r="K31" s="24" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C32" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B32,""\n"",FALSE))"),"Half-Kneeling Windmill")</f>
@@ -6756,20 +6826,20 @@
       <c r="F32" s="23"/>
       <c r="G32" s="23"/>
       <c r="H32" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I32" s="23"/>
       <c r="J32" s="23"/>
       <c r="K32" s="24" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="C33" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B33,""\n"",FALSE))"),"Quarter Turkish Get-Up")</f>
@@ -6786,20 +6856,20 @@
       <c r="F33" s="23"/>
       <c r="G33" s="23"/>
       <c r="H33" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I33" s="23"/>
       <c r="J33" s="23"/>
       <c r="K33" s="24" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="23" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C34" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B34,""\n"",FALSE))"),"Half-Kneeling Clean &amp; Press Windmill")</f>
@@ -6814,24 +6884,24 @@
         <v>C&amp;P, G</v>
       </c>
       <c r="F34" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G34" s="23"/>
       <c r="H34" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I34" s="23"/>
       <c r="J34" s="23"/>
       <c r="K34" s="24" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="23" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C35" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B35,""\n"",FALSE))"),"Half Get-Up")</f>
@@ -6848,20 +6918,20 @@
       <c r="F35" s="23"/>
       <c r="G35" s="23"/>
       <c r="H35" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I35" s="23"/>
       <c r="J35" s="23"/>
       <c r="K35" s="24" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="23" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C36" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B36,""\n"",FALSE))"),"Clean &amp; Press to Overhead Step-Back Lunge")</f>
@@ -6876,24 +6946,24 @@
         <v>C&amp;P, G</v>
       </c>
       <c r="F36" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G36" s="23"/>
       <c r="H36" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I36" s="23"/>
       <c r="J36" s="23"/>
       <c r="K36" s="24" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="23" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C37" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B37,""\n"",FALSE))"),"Half-Kneeling Hip Drop")</f>
@@ -6910,20 +6980,20 @@
       <c r="F37" s="23"/>
       <c r="G37" s="23"/>
       <c r="H37" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I37" s="23"/>
       <c r="J37" s="23"/>
       <c r="K37" s="24" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="23" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C38" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B38,""\n"",FALSE))"),"Half Get-Up to Hip Pass")</f>
@@ -6940,20 +7010,20 @@
       <c r="F38" s="23"/>
       <c r="G38" s="23"/>
       <c r="H38" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I38" s="23"/>
       <c r="J38" s="23"/>
       <c r="K38" s="24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="23" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C39" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B39,""\n"",FALSE))"),"Half-Kneeling Clean &amp; Press to Hip Drop")</f>
@@ -6968,24 +7038,24 @@
         <v>C&amp;P, G</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G39" s="23"/>
       <c r="H39" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I39" s="23"/>
       <c r="J39" s="23"/>
       <c r="K39" s="24" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="23" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C40" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B40,""\n"",FALSE))"),"Box Squat to Boat Pose")</f>
@@ -7003,19 +7073,19 @@
       <c r="G40" s="23"/>
       <c r="H40" s="23"/>
       <c r="I40" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J40" s="23"/>
       <c r="K40" s="24" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="23" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C41" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B41,""\n"",FALSE))"),"Spinal Rock (Bodyweight)")</f>
@@ -7032,22 +7102,22 @@
       <c r="F41" s="23"/>
       <c r="G41" s="23"/>
       <c r="H41" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J41" s="23"/>
       <c r="K41" s="24" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="23" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C42" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B42,""\n"",FALSE))"),"Flat Back Pullover")</f>
@@ -7064,20 +7134,20 @@
       <c r="F42" s="23"/>
       <c r="G42" s="23"/>
       <c r="H42" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I42" s="23"/>
       <c r="J42" s="23"/>
       <c r="K42" s="24" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="23" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C43" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B43,""\n"",FALSE))"),"Half Get-Up to Hip Pass (to Half-Kneeling)")</f>
@@ -7094,20 +7164,20 @@
       <c r="F43" s="23"/>
       <c r="G43" s="23"/>
       <c r="H43" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I43" s="23"/>
       <c r="J43" s="23"/>
       <c r="K43" s="24" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="23" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C44" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B44,""\n"",FALSE))"),"Spinal Rock")</f>
@@ -7124,22 +7194,22 @@
       <c r="F44" s="23"/>
       <c r="G44" s="23"/>
       <c r="H44" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J44" s="23"/>
       <c r="K44" s="24" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="23" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C45" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B45,""\n"",FALSE))"),"Push Press")</f>
@@ -7154,22 +7224,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G45" s="23"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
       <c r="K45" s="24" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="23" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C46" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B46,""\n"",FALSE))"),"Rock-Bottom Curl with Goblet Squat")</f>
@@ -7187,19 +7257,19 @@
       <c r="G46" s="23"/>
       <c r="H46" s="23"/>
       <c r="I46" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J46" s="23"/>
       <c r="K46" s="24" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B47" s="23" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C47" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B47,""\n"",FALSE))"),"Rock-Bottom Front Squat Pickup")</f>
@@ -7217,19 +7287,19 @@
       <c r="G47" s="23"/>
       <c r="H47" s="23"/>
       <c r="I47" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J47" s="23"/>
       <c r="K47" s="24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="23" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C48" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B48,""\n"",FALSE))"),"Thruster")</f>
@@ -7246,20 +7316,20 @@
       <c r="F48" s="23"/>
       <c r="G48" s="23"/>
       <c r="H48" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I48" s="23"/>
       <c r="J48" s="23"/>
       <c r="K48" s="24" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="23" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C49" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B49,""\n"",FALSE))"),"Seated Two-Handed Overhead Press")</f>
@@ -7274,24 +7344,24 @@
         <v>C&amp;P, G</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G49" s="23"/>
       <c r="H49" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I49" s="23"/>
       <c r="J49" s="23"/>
       <c r="K49" s="24" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="23" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B50" s="23" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C50" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B50,""\n"",FALSE))"),"Two-Handed Dead Clean to Double Front Rack")</f>
@@ -7306,22 +7376,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F50" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G50" s="23"/>
       <c r="H50" s="23"/>
       <c r="I50" s="23"/>
       <c r="J50" s="23"/>
       <c r="K50" s="24" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="23" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B51" s="23" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C51" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B51,""\n"",FALSE))"),"Four-Count Squat (Bodyweight)")</f>
@@ -7339,19 +7409,19 @@
       <c r="G51" s="23"/>
       <c r="H51" s="23"/>
       <c r="I51" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J51" s="23"/>
       <c r="K51" s="24" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="23" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C52" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B52,""\n"",FALSE))"),"Rack Alt Shinbox")</f>
@@ -7368,20 +7438,20 @@
       <c r="F52" s="23"/>
       <c r="G52" s="23"/>
       <c r="H52" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I52" s="23"/>
       <c r="J52" s="23"/>
       <c r="K52" s="24" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="23" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C53" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B53,""\n"",FALSE))"),"Handle Up Goblet Squat")</f>
@@ -7399,19 +7469,19 @@
       <c r="G53" s="23"/>
       <c r="H53" s="23"/>
       <c r="I53" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J53" s="23"/>
       <c r="K53" s="24" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="23" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C54" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B54,""\n"",FALSE))"),"Contra Shinbox Press")</f>
@@ -7428,20 +7498,20 @@
       <c r="F54" s="23"/>
       <c r="G54" s="23"/>
       <c r="H54" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I54" s="23"/>
       <c r="J54" s="23"/>
       <c r="K54" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="23" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C55" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B55,""\n"",FALSE))"),"Flat Back Pullover Situp Press")</f>
@@ -7458,20 +7528,20 @@
       <c r="F55" s="23"/>
       <c r="G55" s="23"/>
       <c r="H55" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I55" s="23"/>
       <c r="J55" s="23"/>
       <c r="K55" s="24" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="23" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B56" s="23" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C56" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B56,""\n"",FALSE))"),"Suitcase Deadlift")</f>
@@ -7487,21 +7557,21 @@
       </c>
       <c r="F56" s="23"/>
       <c r="G56" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H56" s="23"/>
       <c r="I56" s="23"/>
       <c r="J56" s="23"/>
       <c r="K56" s="24" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="23" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C57" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B57,""\n"",FALSE))"),"Double Suitcase")</f>
@@ -7517,21 +7587,21 @@
       </c>
       <c r="F57" s="23"/>
       <c r="G57" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H57" s="23"/>
       <c r="I57" s="23"/>
       <c r="J57" s="23"/>
       <c r="K57" s="24" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="23" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B58" s="23" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C58" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B58,""\n"",FALSE))"),"Double Sumo Deadlift")</f>
@@ -7547,21 +7617,21 @@
       </c>
       <c r="F58" s="23"/>
       <c r="G58" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H58" s="23"/>
       <c r="I58" s="23"/>
       <c r="J58" s="23"/>
       <c r="K58" s="24" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="23" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C59" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B59,""\n"",FALSE))"),"Half Snatch Down")</f>
@@ -7576,22 +7646,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G59" s="23"/>
       <c r="H59" s="23"/>
       <c r="I59" s="23"/>
       <c r="J59" s="23"/>
       <c r="K59" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="23" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C60" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B60,""\n"",FALSE))"),"Double Swing")</f>
@@ -7606,24 +7676,24 @@
         <v>C&amp;P, Sw</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H60" s="23"/>
       <c r="I60" s="23"/>
       <c r="J60" s="23"/>
       <c r="K60" s="24" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="23" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B61" s="23" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C61" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B61,""\n"",FALSE))"),"Half Snatch Up")</f>
@@ -7638,22 +7708,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F61" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G61" s="23"/>
       <c r="H61" s="23"/>
       <c r="I61" s="23"/>
       <c r="J61" s="23"/>
       <c r="K61" s="24" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="23" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C62" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B62,""\n"",FALSE))"),"Double Clean")</f>
@@ -7668,22 +7738,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F62" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G62" s="23"/>
       <c r="H62" s="23"/>
       <c r="I62" s="23"/>
       <c r="J62" s="23"/>
       <c r="K62" s="24" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="23" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C63" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B63,""\n"",FALSE))"),"Double Rockit")</f>
@@ -7702,18 +7772,18 @@
       <c r="H63" s="23"/>
       <c r="I63" s="23"/>
       <c r="J63" s="23" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="K63" s="24" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="23" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C64" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B64,""\n"",FALSE))"),"Double Outside Swing")</f>
@@ -7729,21 +7799,21 @@
       </c>
       <c r="F64" s="23"/>
       <c r="G64" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H64" s="23"/>
       <c r="I64" s="23"/>
       <c r="J64" s="23"/>
       <c r="K64" s="24" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="23" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C65" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B65,""\n"",FALSE))"),"Double Clean &amp; Press")</f>
@@ -7758,22 +7828,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F65" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G65" s="23"/>
       <c r="H65" s="23"/>
       <c r="I65" s="23"/>
       <c r="J65" s="23"/>
       <c r="K65" s="24" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="23" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C66" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B66,""\n"",FALSE))"),"Full Snatch")</f>
@@ -7788,22 +7858,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F66" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G66" s="23"/>
       <c r="H66" s="23"/>
       <c r="I66" s="23"/>
       <c r="J66" s="23"/>
       <c r="K66" s="24" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="23" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B67" s="23" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="C67" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B67,""\n"",FALSE))"),"Double Front Squat")</f>
@@ -7821,19 +7891,19 @@
       <c r="G67" s="23"/>
       <c r="H67" s="23"/>
       <c r="I67" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J67" s="23"/>
       <c r="K67" s="24" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="23" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C68" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B68,""\n"",FALSE))"),"Double Clean to Front Squat")</f>
@@ -7848,24 +7918,24 @@
         <v>C&amp;P, Sq</v>
       </c>
       <c r="F68" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G68" s="23"/>
       <c r="H68" s="23"/>
       <c r="I68" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J68" s="23"/>
       <c r="K68" s="24" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="23" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C69" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B69,""\n"",FALSE))"),"Snatch Press")</f>
@@ -7880,22 +7950,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F69" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G69" s="23"/>
       <c r="H69" s="23"/>
       <c r="I69" s="23"/>
       <c r="J69" s="23"/>
       <c r="K69" s="24" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="23" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="B70" s="23" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C70" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B70,""\n"",FALSE))"),"Half-Kneeling Snatch Up")</f>
@@ -7910,24 +7980,24 @@
         <v>C&amp;P, G</v>
       </c>
       <c r="F70" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G70" s="23"/>
       <c r="H70" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I70" s="23"/>
       <c r="J70" s="23"/>
       <c r="K70" s="24" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="23" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C71" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B71,""\n"",FALSE))"),"Dead Stop Double Clean")</f>
@@ -7942,22 +8012,22 @@
         <v>C&amp;P</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G71" s="23"/>
       <c r="H71" s="23"/>
       <c r="I71" s="23"/>
       <c r="J71" s="23"/>
       <c r="K71" s="24" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="23" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B72" s="23" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C72" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B72,""\n"",FALSE))"),"Deck Squat")</f>
@@ -7974,22 +8044,22 @@
       <c r="F72" s="23"/>
       <c r="G72" s="23"/>
       <c r="H72" s="23" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J72" s="23"/>
       <c r="K72" s="24" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="23" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C73" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B73,""\n"",FALSE))"),"Two Hand Single Bent Leg Deadlift")</f>
@@ -8005,21 +8075,21 @@
       </c>
       <c r="F73" s="23"/>
       <c r="G73" s="23" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H73" s="23"/>
       <c r="I73" s="23"/>
       <c r="J73" s="23"/>
       <c r="K73" s="24" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="23" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C74" s="23" t="str">
         <f aca="false">IFERROR(__xludf.dummyfunction("Textjoin("" "",TRUE,split(B74,""\n"",FALSE))"),"Double Hang Clean To Squat")</f>
@@ -8034,16 +8104,16 @@
         <v>C&amp;P, Sq</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G74" s="23"/>
       <c r="H74" s="23"/>
       <c r="I74" s="23" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J74" s="23"/>
       <c r="K74" s="24" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>